<commit_message>
Apkopots par jaunajiem failiem.
</commit_message>
<xml_diff>
--- a/Docs/SENIE-kodi-no-ASCII-datiem.xlsx
+++ b/Docs/SENIE-kodi-no-ASCII-datiem.xlsx
@@ -16,26 +16,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
   <si>
     <t>Elg1621_GCG, Manc1631_LVM, Manc1638_L, Manc1638_PhL, Manc1638_Run, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr</t>
   </si>
   <si>
-    <t>Manc1631_LVM, VLH1685_Sal, VLH1685_Syr</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
-    <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Bar, Apokr1689/Bel, Apokr1689/GabpEst, Apokr1689/Jd, Apokr1689/P_Sir, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Sus, Apokr1689/Tit, Apokr1689/Tob, Baum1699_LVV, Baumb1795_WLWJD, Bluhm1791_MWU, Br1520_PN, Bruehn1756_DLWS, CC1585, CekFJ1790_KD, CekFV1796_NL, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Eid1701_KB, Eid1701_RA, Elg1621_GCG, Ench1586, Ench1615, EvEp1587, EvEp1615, EvTA1753, Fuer1650_70_1ms, Fuer1650_70_2ms, Fuhr1690_LL, GD_1698, Gis1507_PN, Gr1520_PN, Hag1790_IM, Has1550_PN, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Rm, JT1685/Tit, LGL1685_K1, LGL1685_V5, LS1625, Laz1557_PN, Lod1775_SEAPP, Lod1778_WTMD, Lop1800_SDLS, MD1788, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Meg1593_PN, Ps1615, Rav1767_SD, Reit1675_OD, Reit1675_UeP, SKL1696_KB, SKL1696_RA, SL1684, SL1789, SLM1648, StendAJ1790_LSMP, StendAJ1793_JGW, StendGF1781_JGW, StendGF1789_SL, Stobbe1796_PTK, Sulc1764_ARMST, TII1790, Tetsch1784_DKTW, Thev1575_PN, UP1587, Urban1791_LKLDD, V1771_SZA, VD1689_94/1Ken, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr, Witt1696_MMID, Witt1702_PAN, ZP1685, Zv1638_VAR, Zv1681_Kok, Zv1681_Liec_1, Zv1681_Liec_2, Zv1689_Kan, Zv1689_Salsnes, Zv1698_Lig</t>
-  </si>
-  <si>
     <t>b</t>
   </si>
   <si>
-    <t>CC1585, CekFJ1790_KD, CekFV1796_NL, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Eid1701_KB, Ench1586, Ench1615, EvEp1587, EvEp1615, EvTA1753, Fuhr1690_LL, GD_1698, Hag1790_IM, LGL1685_K1, LGL1685_V5, Lod1775_SEAPP, Lod1778_WTMD, Lop1800_SDLS, MD1788, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Ps1615, Rav1767_SD, Reit1675_UeP, SKL1696_KB, SL1684, SL1789, StendAJ1790_LSMP, StendGF1789_SL, Sulc1764_ARMST, TII1790, UP1587, Urban1791_LKLDD, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr</t>
-  </si>
-  <si>
     <t>c</t>
   </si>
   <si>
@@ -63,36 +54,21 @@
     <t>g</t>
   </si>
   <si>
-    <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Bar, Apokr1689/Bel, Apokr1689/GabpEst, Apokr1689/Jd, Apokr1689/P_Sir, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Sus, Apokr1689/Tit, Apokr1689/Tob, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Rm, JT1685/Tit, VD1689_94/1Ken, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
-  </si>
-  <si>
     <t>h</t>
   </si>
   <si>
-    <t>Depk1704_Vortr, Fuer1650_70_1ms, Manc1631_Cat, Manc1631_LVM, Manc1631_Syr</t>
-  </si>
-  <si>
     <t>i</t>
   </si>
   <si>
     <t>k</t>
   </si>
   <si>
-    <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Bar, Apokr1689/Bel, Apokr1689/GabpEst, Apokr1689/Jd, Apokr1689/P_Sir, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Sus, Apokr1689/Tob, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Rm, JT1685/Tit, VD1689_94/1Ken, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
-  </si>
-  <si>
     <t>l</t>
   </si>
   <si>
-    <t>Apokr1689/Sal, Br1520_PN, CC1585, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Elg1621_GCG, Ench1586, Ench1615, EvEp1587, EvEp1615, EvTA1753, Fuer1650_70_1ms, Fuer1650_70_2ms, GD_1698, JT1685/Lk, JT1685/Mk, JT1685/Mt, LGL1685_K1, LGL1685_V5, Lop1800_SDLS, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Meg1593_PN, Ps1615, Reit1675_OD, Reit1675_UeP, SL1684, SLM1648, StendAJ1793_JGW, UP1587, V1771_SZA, VD1689_94/1Ken, VD1689_94/2L, VD1689_94/2Sam, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Ech, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hoz, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ps, VD1689_94/Sak, VD1689_94/Zah, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr, Witt1702_PAN, Zv1681_Kok, Zv1681_Liec_1, Zv1689_Kan, Zv1698_Lig</t>
-  </si>
-  <si>
     <t>n</t>
   </si>
   <si>
-    <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Bar, Apokr1689/Bel, Apokr1689/GabpEst, Apokr1689/Jd, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Sus, Apokr1689/Tob, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Rm, JT1685/Tit, VD1689_94/1Ken, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
-  </si>
-  <si>
     <t>o</t>
   </si>
   <si>
@@ -102,30 +78,18 @@
     <t>p</t>
   </si>
   <si>
-    <t>Apokr1689/2Mak, Apokr1689/Sir, JT1685/1Kor, JT1685/Apd, JT1685/Ef, JT1685/Jn, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Rm, LGL1685_V5, Manc1631_LVM, Manc1637_Sal, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, VD1689_94/1Ken, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
-  </si>
-  <si>
     <t>r</t>
   </si>
   <si>
-    <t>EvEp1615, VLH1685</t>
-  </si>
-  <si>
     <t>s</t>
   </si>
   <si>
     <t>t</t>
   </si>
   <si>
-    <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Bar, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Tob, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Rm, JT1685/Tit, Lod1775_SEAPP, VD1689_94/1Ken, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
-  </si>
-  <si>
     <t>v</t>
   </si>
   <si>
-    <t>Baum1699_LVV, Baumb1795_WLWJD, CC1585, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Eid1701_KB, Eid1701_RA, Elg1621_GCG, Ench1586, Ench1615, EvEp1587, EvEp1615, Fuer1650_70_1ms, Fuer1650_70_2ms, Hag1790_IM, LGL1685_K1, LGL1685_V5, LS1625, Lod1778_WTMD, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Ps1615, SKL1696_KB, SL1684, StendAJ1790_LSMP, StendGF1789_SL, UP1587, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr, Witt1702_PAN, Zv1638_VAR, Zv1681_Kok, Zv1681_Liec_1, Zv1681_Liec_2, Zv1689_Kan, Zv1689_Salsnes, Zv1698_Lig</t>
-  </si>
-  <si>
     <t>z</t>
   </si>
   <si>
@@ -229,6 +193,45 @@
   </si>
   <si>
     <t>Piezīmes par indeksāciju</t>
+  </si>
+  <si>
+    <t>Manc1631_LVM, Manc1643_44_LVM, Manc1643_LGL, Manc1643_Syr, VLH1685_Sal, VLH1685_Syr</t>
+  </si>
+  <si>
+    <t>Manc1631_LVM, Manc1643_LGL, Manc1643_Syr, VLH1685_Sal, VLH1685_Syr</t>
+  </si>
+  <si>
+    <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Bar, Apokr1689/Bel, Apokr1689/GabpEst, Apokr1689/Jd, Apokr1689/P_Sir, Apokr1689/Prolog, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Sus, Apokr1689/Tob, Baum1699_LVV, Baumb1795_WLWJD, Bluhm1791_MWU, Br1520_PN, Bruehn1756_DLWS, CC1585, CekFJ1790_KD, CekFV1796_NL, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Eid1701_KB, Eid1701_RA, Elg1621_GCG, Ench1586, Ench1615, EvEp1587, EvEp1615, EvTA1753, Fuer1650_70_1ms, Fuer1650_70_2ms, Fuhr1690_LL, GD_1698, Gis1507_PN, Gr1520_PN, Hag1790_IM, Has1550_PN, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Prolog_Iev, JT1685/Prolog_Sat, JT1685/Prolog_Tit, JT1685/Rm, JT1685/Tit, LGL1685_K1, LGL1685_V5, LS1625, Laz1557_PN, Lod1775_SEAPP, Lod1778_WTMD, Lop1800_SDLS, MD1788, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1643_44_Cat, Manc1643_44_LVM, Manc1643_LGL, Manc1643_Syr, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Meg1593_PN, Ps1615, Rav1767_SD, Reit1675_OD, Reit1675_UeP, SKL1696_KB, SKL1696_RA, SL1684, SL1789, SLM1648, StendAJ1790_LSMP, StendAJ1793_JGW, StendGF1781_JGW, StendGF1789_SL, Stobbe1796_PTK, Sulc1764_ARMST, TII1790, Tetsch1784_DKTW, Thev1575_PN, UP1587, Urban1791_LKLDD, V1771_SZA, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr, Witt1696_MMID, Witt1702_PAN, ZP1685, Zv1638_VAR, Zv1681_Kok, Zv1681_Liec_1, Zv1681_Liec_2, Zv1689_Kan, Zv1689_Salsnes, Zv1698_Lig</t>
+  </si>
+  <si>
+    <t>CC1585, CekFJ1790_KD, CekFV1796_NL, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Eid1701_KB, Ench1586, Ench1615, EvEp1587, EvEp1615, EvTA1753, Fuhr1690_LL, GD_1698, Hag1790_IM, JT1685/Prolog_Iev, LGL1685_K1, LGL1685_V5, Lod1775_SEAPP, Lod1778_WTMD, Lop1800_SDLS, MD1788, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1643_44_Cat, Manc1643_44_LVM, Manc1643_LGL, Manc1643_Syr, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Ps1615, Rav1767_SD, Reit1675_UeP, SKL1696_KB, SL1684, SL1789, StendAJ1790_LSMP, StendGF1789_SL, Sulc1764_ARMST, TII1790, UP1587, Urban1791_LKLDD, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr</t>
+  </si>
+  <si>
+    <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Bar, Apokr1689/Bel, Apokr1689/GabpEst, Apokr1689/Jd, Apokr1689/P_Sir, Apokr1689/Prolog, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Sus, Apokr1689/Tob, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Prolog_Iev, JT1685/Prolog_Sat, JT1685/Prolog_Tit, JT1685/Rm, JT1685/Tit, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
+  </si>
+  <si>
+    <t>Depk1704_Vortr, Fuer1650_70_1ms, Manc1631_Cat, Manc1631_LVM, Manc1631_Syr, Manc1643_44_Cat, Manc1643_44_LVM</t>
+  </si>
+  <si>
+    <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Bar, Apokr1689/Bel, Apokr1689/GabpEst, Apokr1689/Jd, Apokr1689/P_Sir, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Sus, Apokr1689/Tob, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Rm, JT1685/Tit, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
+  </si>
+  <si>
+    <t>Apokr1689/Sal, Br1520_PN, CC1585, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Elg1621_GCG, Ench1586, Ench1615, EvEp1587, EvEp1615, EvTA1753, Fuer1650_70_1ms, Fuer1650_70_2ms, GD_1698, JT1685/1Kor, JT1685/1P, JT1685/2Kor, JT1685/Atk, JT1685/Jk, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Prolog_Tit, JT1685/Rm, LGL1685_K1, LGL1685_V5, Lop1800_SDLS, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1643_44_Cat, Manc1643_44_LVM, Manc1643_LGL, Manc1643_Syr, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Meg1593_PN, Ps1615, Reit1675_OD, Reit1675_UeP, SL1684, SLM1648, StendAJ1793_JGW, UP1587, V1771_SZA, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/2L, VD1689_94/2Sam, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Ech, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Mac, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ps, VD1689_94/Sak, VD1689_94/Zah, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr, Witt1702_PAN, Zv1681_Kok, Zv1681_Liec_1, Zv1689_Kan, Zv1698_Lig</t>
+  </si>
+  <si>
+    <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Bar, Apokr1689/Bel, Apokr1689/GabpEst, Apokr1689/Jd, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Sus, Apokr1689/Tob, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Rm, JT1685/Tit, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
+  </si>
+  <si>
+    <t>Apokr1689/2Mak, Apokr1689/Sir, JT1685/Apd, JT1685/Ef, JT1685/Jn, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Prolog_Iev, JT1685/Rm, LGL1685_V5, Manc1631_LVM, Manc1637_Sal, Manc1643_44_LVM, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
+  </si>
+  <si>
+    <t>EvEp1615, JT1685/Mk, Manc1643_44_LVM, Manc1643_LGL, VLH1685</t>
+  </si>
+  <si>
+    <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Bar, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Tob, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Rm, JT1685/Tit, Lod1775_SEAPP, Manc1643_44_LVM, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
+  </si>
+  <si>
+    <t>Baum1699_LVV, Baumb1795_WLWJD, CC1585, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Eid1701_KB, Eid1701_RA, Elg1621_GCG, Ench1586, Ench1615, EvEp1587, EvEp1615, Fuer1650_70_1ms, Fuer1650_70_2ms, Hag1790_IM, JT1685/Prolog_Iev, JT1685/Prolog_Tit, LGL1685_K1, LGL1685_V5, LS1625, Lod1778_WTMD, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1643_44_Cat, Manc1643_44_LVM, Manc1643_LGL, Manc1643_Syr, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Ps1615, SKL1696_KB, SL1684, StendAJ1790_LSMP, StendGF1789_SL, UP1587, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr, Witt1702_PAN, Zv1638_VAR, Zv1681_Kok, Zv1681_Liec_1, Zv1681_Liec_2, Zv1689_Kan, Zv1689_Salsnes, Zv1698_Lig</t>
   </si>
 </sst>
 </file>
@@ -608,7 +611,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,22 +626,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -649,10 +652,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -660,13 +663,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -674,228 +677,228 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="330" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="315" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="B12" s="2" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="315" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="330" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Precizējumi par veco indeksēšanu un jauno transliterēšanu.
</commit_message>
<xml_diff>
--- a/Docs/SENIE-kodi-no-ASCII-datiem.xlsx
+++ b/Docs/SENIE-kodi-no-ASCII-datiem.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="80">
   <si>
     <t>Elg1621_GCG, Manc1631_LVM, Manc1638_L, Manc1638_PhL, Manc1638_Run, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr</t>
   </si>
@@ -241,6 +241,21 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>Nē</t>
+  </si>
+  <si>
+    <t>Jā</t>
+  </si>
+  <si>
+    <t>Kaut kādi tukšumi?</t>
+  </si>
+  <si>
+    <t>Nē (Normunds)</t>
+  </si>
+  <si>
+    <t>Vai mūsdienīgo?</t>
   </si>
 </sst>
 </file>
@@ -616,24 +631,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="109.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="109.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
@@ -644,16 +662,19 @@
         <v>52</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -663,11 +684,17 @@
       <c r="C2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="D2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -677,11 +704,17 @@
       <c r="C3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="D3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -691,11 +724,17 @@
       <c r="C4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="D4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="330" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="330" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
@@ -705,8 +744,11 @@
       <c r="C5" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -716,8 +758,14 @@
       <c r="C6" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -727,8 +775,14 @@
       <c r="C7" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -738,8 +792,14 @@
       <c r="C8" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -749,8 +809,14 @@
       <c r="C9" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -760,8 +826,14 @@
       <c r="C10" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="D10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -771,8 +843,11 @@
       <c r="C11" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D11" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -782,8 +857,14 @@
       <c r="C12" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -793,13 +874,22 @@
       <c r="C13" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="E14" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -809,8 +899,14 @@
       <c r="C15" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="D15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -820,8 +916,14 @@
       <c r="C16" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="D16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -831,13 +933,19 @@
       <c r="C17" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D17" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="E18" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -847,16 +955,22 @@
       <c r="C19" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="D19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -866,8 +980,14 @@
       <c r="C21" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D21" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -877,8 +997,14 @@
       <c r="C22" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="D22" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
@@ -888,13 +1014,19 @@
       <c r="C23" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D23" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>22</v>
       </c>
@@ -904,23 +1036,38 @@
       <c r="C25" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C27" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="330" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="318" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>23</v>
       </c>
@@ -929,6 +1076,9 @@
       </c>
       <c r="C29" s="2" t="s">
         <v>50</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Precizējumi no Everitas par kodiem.
</commit_message>
<xml_diff>
--- a/Docs/SENIE-kodi-no-ASCII-datiem.xlsx
+++ b/Docs/SENIE-kodi-no-ASCII-datiem.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everita\Documents\Everita-2019Nov\Kopija_24novembris2019\Senie_2019\DigHuman_VPP\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6470"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="89">
   <si>
     <t>Elg1621_GCG, Manc1631_LVM, Manc1638_L, Manc1638_PhL, Manc1638_Run, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr</t>
   </si>
@@ -249,19 +254,46 @@
     <t>Jā</t>
   </si>
   <si>
-    <t>Kaut kādi tukšumi?</t>
-  </si>
-  <si>
     <t>Nē (Normunds)</t>
   </si>
   <si>
     <t>Vai mūsdienīgo?</t>
+  </si>
+  <si>
+    <t>Nē, neindeksē (Everita)</t>
+  </si>
+  <si>
+    <t>Tas bija vecais, tikai vienā avotā izmantototais apzīmējums nodaļas nosaukumam augšā, kas atkārtojas katrā lapā. Šobrīd mēs to vairs neizmantojam.</t>
+  </si>
+  <si>
+    <t>Brīvs :-)</t>
+  </si>
+  <si>
+    <t>Kaut kādi tukšumi? - Tas varētu būt izmantots xxx kā kaut kas nesalasāms, bet vai tas patiešām ir iekš {} ?</t>
+  </si>
+  <si>
+    <t>Nē (Everita)</t>
+  </si>
+  <si>
+    <t>manuprāt, brīvs apzīmējums :)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nē, neindeksē (Everita). </t>
+  </si>
+  <si>
+    <t>Everita: Teorētiski tas arī ir teksts latviski, tāpēc, ja ir vēlme, to varētu indeksēt, bet adresē tad norādītu tikai, piem., JT1685 2P_g - bet tas tad būtu jāatrunā. Šobrīd mums jau ir 0. pants, ko mēs indeksējam, kas arī nav "oficiālais" Bībeles teksts. Bet šis @g{} ir nesvarīgs, tāpēc mēs varam turpināt to ignorēt. Piemēram @p{} ir daudz svarīgāks, ko vajadzētu indeksēt. sk. zemāk</t>
+  </si>
+  <si>
+    <t>Everita:  ja ir iespēja, tad mēs ļoti gribētu šīs Bībeles (!) piezīmes tekstu arī indeksēt, jo tas ir latviski. Adrese šādam vārdlietojumam būtu tāds pat kā Bībelei: nodaļa: pants+p , piem., kaut kāds (izgudrots piemērs) 1Sam 1:4p. Savukārt tur, kur piezīme ir ne Bībeles tekstā, to var ignorēt, jo tas ir tikai atsevišķš vārds vai skaņa, kurai turklāt grūti "pielikt" adresi (precīzu rindiņu), labākajā gadījumā tā ir tikai lappuses p: Manc1631_LVM 12p (izdomāts piemērs) -- bet tas lec ārā no pārējās šī avota adreses. Ne Bībeles tekstā šis ir mazsvarīgs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nē (Normunds). </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -387,7 +419,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -422,7 +454,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -634,24 +666,24 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="109.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="5.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="109.81640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.81640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.26953125" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
@@ -662,7 +694,7 @@
         <v>52</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>54</v>
@@ -674,7 +706,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -688,13 +720,13 @@
         <v>75</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -708,13 +740,13 @@
         <v>76</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -728,13 +760,13 @@
         <v>76</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="330" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
@@ -747,8 +779,11 @@
       <c r="D5" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -762,10 +797,10 @@
         <v>75</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -779,10 +814,10 @@
         <v>75</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -796,10 +831,10 @@
         <v>75</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -813,10 +848,10 @@
         <v>75</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -830,10 +865,10 @@
         <v>75</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -846,8 +881,14 @@
       <c r="D11" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -861,10 +902,10 @@
         <v>75</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -878,18 +919,21 @@
         <v>75</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>69</v>
       </c>
+      <c r="C14" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E14" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="152.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -903,10 +947,10 @@
         <v>76</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -920,10 +964,10 @@
         <v>75</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -936,16 +980,22 @@
       <c r="D17" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E17" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="C18" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="E18" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -959,18 +1009,24 @@
         <v>76</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>78</v>
+        <v>88</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -984,10 +1040,10 @@
         <v>75</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -1001,10 +1057,10 @@
         <v>75</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
@@ -1018,15 +1074,18 @@
         <v>76</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="C24" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>22</v>
       </c>
@@ -1040,34 +1099,37 @@
         <v>75</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>75</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="318" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="318" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>23</v>
       </c>
@@ -1078,6 +1140,9 @@
         <v>50</v>
       </c>
       <c r="D29" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1093,7 +1158,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1105,7 +1170,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Atjauninātas indeksu sastopamības vietas pēc failu pārdalīšanas.
</commit_message>
<xml_diff>
--- a/Docs/SENIE-kodi-no-ASCII-datiem.xlsx
+++ b/Docs/SENIE-kodi-no-ASCII-datiem.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="91">
   <si>
     <t>Elg1621_GCG, Manc1631_LVM, Manc1638_L, Manc1638_PhL, Manc1638_Run, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr</t>
   </si>
@@ -186,27 +186,9 @@
     <t>Piezīmes par indeksāciju</t>
   </si>
   <si>
-    <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Bar, Apokr1689/Bel, Apokr1689/GabpEst, Apokr1689/Jd, Apokr1689/P_Sir, Apokr1689/Prolog, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Sus, Apokr1689/Tob, Baum1699_LVV, Baumb1795_WLWJD, Bluhm1791_MWU, Br1520_PN, Bruehn1756_DLWS, CC1585, CekFJ1790_KD, CekFV1796_NL, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Eid1701_KB, Eid1701_RA, Elg1621_GCG, Ench1586, Ench1615, EvEp1587, EvEp1615, EvTA1753, Fuer1650_70_1ms, Fuer1650_70_2ms, Fuhr1690_LL, GD_1698, Gis1507_PN, Gr1520_PN, Hag1790_IM, Has1550_PN, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Prolog_Iev, JT1685/Prolog_Sat, JT1685/Prolog_Tit, JT1685/Rm, JT1685/Tit, LGL1685_K1, LGL1685_V5, LS1625, Laz1557_PN, Lod1775_SEAPP, Lod1778_WTMD, Lop1800_SDLS, MD1788, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1643_44_Cat, Manc1643_44_LVM, Manc1643_LGL, Manc1643_Syr, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Meg1593_PN, Ps1615, Rav1767_SD, Reit1675_OD, Reit1675_UeP, SKL1696_KB, SKL1696_RA, SL1684, SL1789, SLM1648, StendAJ1790_LSMP, StendAJ1793_JGW, StendGF1781_JGW, StendGF1789_SL, Stobbe1796_PTK, Sulc1764_ARMST, TII1790, Tetsch1784_DKTW, Thev1575_PN, UP1587, Urban1791_LKLDD, V1771_SZA, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr, Witt1696_MMID, Witt1702_PAN, ZP1685, Zv1638_VAR, Zv1681_Kok, Zv1681_Liec_1, Zv1681_Liec_2, Zv1689_Kan, Zv1689_Salsnes, Zv1698_Lig</t>
-  </si>
-  <si>
-    <t>CC1585, CekFJ1790_KD, CekFV1796_NL, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Eid1701_KB, Ench1586, Ench1615, EvEp1587, EvEp1615, EvTA1753, Fuhr1690_LL, GD_1698, Hag1790_IM, JT1685/Prolog_Iev, LGL1685_K1, LGL1685_V5, Lod1775_SEAPP, Lod1778_WTMD, Lop1800_SDLS, MD1788, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1643_44_Cat, Manc1643_44_LVM, Manc1643_LGL, Manc1643_Syr, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Ps1615, Rav1767_SD, Reit1675_UeP, SKL1696_KB, SL1684, SL1789, StendAJ1790_LSMP, StendGF1789_SL, Sulc1764_ARMST, TII1790, UP1587, Urban1791_LKLDD, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr</t>
-  </si>
-  <si>
-    <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Bar, Apokr1689/Bel, Apokr1689/GabpEst, Apokr1689/Jd, Apokr1689/P_Sir, Apokr1689/Prolog, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Sus, Apokr1689/Tob, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Prolog_Iev, JT1685/Prolog_Sat, JT1685/Prolog_Tit, JT1685/Rm, JT1685/Tit, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
-  </si>
-  <si>
     <t>Depk1704_Vortr, Fuer1650_70_1ms, Manc1631_Cat, Manc1631_LVM, Manc1631_Syr, Manc1643_44_Cat, Manc1643_44_LVM</t>
   </si>
   <si>
-    <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Bar, Apokr1689/Bel, Apokr1689/GabpEst, Apokr1689/Jd, Apokr1689/P_Sir, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Sus, Apokr1689/Tob, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Rm, JT1685/Tit, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
-  </si>
-  <si>
-    <t>Apokr1689/Sal, Br1520_PN, CC1585, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Elg1621_GCG, Ench1586, Ench1615, EvEp1587, EvEp1615, EvTA1753, Fuer1650_70_1ms, Fuer1650_70_2ms, GD_1698, JT1685/1Kor, JT1685/1P, JT1685/2Kor, JT1685/Atk, JT1685/Jk, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Prolog_Tit, JT1685/Rm, LGL1685_K1, LGL1685_V5, Lop1800_SDLS, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1643_44_Cat, Manc1643_44_LVM, Manc1643_LGL, Manc1643_Syr, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Meg1593_PN, Ps1615, Reit1675_OD, Reit1675_UeP, SL1684, SLM1648, StendAJ1793_JGW, UP1587, V1771_SZA, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/2L, VD1689_94/2Sam, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Ech, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Mac, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ps, VD1689_94/Sak, VD1689_94/Zah, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr, Witt1702_PAN, Zv1681_Kok, Zv1681_Liec_1, Zv1689_Kan, Zv1698_Lig</t>
-  </si>
-  <si>
-    <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Bar, Apokr1689/Bel, Apokr1689/GabpEst, Apokr1689/Jd, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Sus, Apokr1689/Tob, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Rm, JT1685/Tit, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
-  </si>
-  <si>
     <t>Apokr1689/2Mak, Apokr1689/Sir, JT1685/Apd, JT1685/Ef, JT1685/Jn, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Prolog_Iev, JT1685/Rm, LGL1685_V5, Manc1631_LVM, Manc1637_Sal, Manc1643_44_LVM, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
   </si>
   <si>
@@ -216,9 +198,6 @@
     <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Bar, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Tob, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Rm, JT1685/Tit, Lod1775_SEAPP, Manc1643_44_LVM, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
   </si>
   <si>
-    <t>Baum1699_LVV, Baumb1795_WLWJD, CC1585, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Eid1701_KB, Eid1701_RA, Elg1621_GCG, Ench1586, Ench1615, EvEp1587, EvEp1615, Fuer1650_70_1ms, Fuer1650_70_2ms, Hag1790_IM, JT1685/Prolog_Iev, JT1685/Prolog_Tit, LGL1685_K1, LGL1685_V5, LS1625, Lod1778_WTMD, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1643_44_Cat, Manc1643_44_LVM, Manc1643_LGL, Manc1643_Syr, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Ps1615, SKL1696_KB, SL1684, StendAJ1790_LSMP, StendGF1789_SL, UP1587, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr, Witt1702_PAN, Zv1638_VAR, Zv1681_Kok, Zv1681_Liec_1, Zv1681_Liec_2, Zv1689_Kan, Zv1689_Salsnes, Zv1698_Lig</t>
-  </si>
-  <si>
     <t>Manc1631_LVM, Manc1643_44_LVM, Manc1643_LGL, Manc1643_Syr, Rav1767_SD, VLH1685_Sal, VLH1685_Syr</t>
   </si>
   <si>
@@ -264,9 +243,6 @@
     <t>Brīvs :-)</t>
   </si>
   <si>
-    <t>Kaut kādi tukšumi? - Tas varētu būt izmantots xxx kā kaut kas nesalasāms, bet vai tas patiešām ir iekš {} ?</t>
-  </si>
-  <si>
     <t>Nē (Everita)</t>
   </si>
   <si>
@@ -283,6 +259,36 @@
   </si>
   <si>
     <t xml:space="preserve">Nē (Normunds). </t>
+  </si>
+  <si>
+    <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Asar, Apokr1689/Bar, Apokr1689/Bel, Apokr1689/GabpEst, Apokr1689/Jd, Apokr1689/Man, Apokr1689/P_Sir, Apokr1689/Prolog, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Sus, Apokr1689/Tob, Baum1699_LVV, Baumb1795_WLWJD, Bluhm1791_MWU, Br1520_PN, Bruehn1756_DLWS, CC1585, CekFJ1790_KD, CekFV1796_NL, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Eid1701_KB, Eid1701_RA, Elg1621_GCG, Ench1586, Ench1615, EvEp1587, EvEp1615, EvTA1753, Fuer1650_70_1ms, Fuer1650_70_2ms, Fuhr1690_LL, GD_1698, Gis1507_PN, Glueck1699_SBM, Gr1520_PN, Hag1790_IM, Has1550_PN, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Prolog_Iev, JT1685/Prolog_Sat, JT1685/Prolog_Tit, JT1685/Rm, JT1685/Tit, LGL1685_K1, LGL1685_V5, LS1625, Laz1557_PN, Lod1775_SEAPP, Lod1778_WTMD, Lop1800_SDLS, MD1788, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1643_44_Cat, Manc1643_44_LVM, Manc1643_LGL, Manc1643_Syr, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Meg1593_PN, Ps1615, Rav1767_SD, Reit1675_OD, Reit1675_UeP, SKL1696_KB, SKL1696_RA, SL1684, SL1789, SLM1648, StendAJ1790_LSMP, StendAJ1793_JGW, StendGF1781_JGW, StendGF1789_SL, Stobbe1796_PTK, Sulc1764_ARMST, TII1790, Tetsch1784_DKTW, Thev1575_PN, UP1587, Urban1791_LKLDD, V1771_SZA, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Prolog, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr, Witt1696_MMID, Witt1702_PAN, ZP1685, Zv1638_VAR, Zv1681_Kok, Zv1681_Liec_1, Zv1681_Liec_2, Zv1689_Kan, Zv1689_Salsnes, Zv1698_Lig</t>
+  </si>
+  <si>
+    <t>CC1585, CekFJ1790_KD, CekFV1796_NL, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Eid1701_KB, Ench1586, Ench1615, EvEp1587, EvEp1615, EvTA1753, Fuhr1690_LL, GD_1698, Glueck1699_SBM, Hag1790_IM, JT1685/Prolog_Iev, LGL1685_K1, LGL1685_V5, Lod1775_SEAPP, Lod1778_WTMD, Lop1800_SDLS, MD1788, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1643_44_Cat, Manc1643_44_LVM, Manc1643_LGL, Manc1643_Syr, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Ps1615, Rav1767_SD, Reit1675_UeP, SKL1696_KB, SL1684, SL1789, StendAJ1790_LSMP, StendGF1789_SL, Sulc1764_ARMST, TII1790, UP1587, Urban1791_LKLDD, VD1689_94/Prolog, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr</t>
+  </si>
+  <si>
+    <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Asar, Apokr1689/Bar, Apokr1689/Bel, Apokr1689/GabpEst, Apokr1689/Jd, Apokr1689/Man, Apokr1689/P_Sir, Apokr1689/Prolog, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Sus, Apokr1689/Tob, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Prolog_Iev, JT1685/Prolog_Sat, JT1685/Prolog_Tit, JT1685/Rm, JT1685/Tit, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Prolog, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
+  </si>
+  <si>
+    <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Asar, Apokr1689/Bar, Apokr1689/Bel, Apokr1689/GabpEst, Apokr1689/Jd, Apokr1689/Man, Apokr1689/P_Sir, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Sus, Apokr1689/Tob, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Rm, JT1685/Tit, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
+  </si>
+  <si>
+    <t>Apokr1689/Sal, Br1520_PN, CC1585, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Elg1621_GCG, Ench1586, Ench1615, EvEp1587, EvEp1615, EvTA1753, Fuer1650_70_1ms, Fuer1650_70_2ms, GD_1698, Glueck1699_SBM, JT1685/1Kor, JT1685/1P, JT1685/2Kor, JT1685/Atk, JT1685/Jk, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Prolog_Tit, JT1685/Rm, LGL1685_K1, LGL1685_V5, Lop1800_SDLS, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1643_44_Cat, Manc1643_44_LVM, Manc1643_LGL, Manc1643_Syr, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Meg1593_PN, Ps1615, Reit1675_OD, Reit1675_UeP, SL1684, SLM1648, StendAJ1793_JGW, UP1587, V1771_SZA, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/2L, VD1689_94/2Sam, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Ech, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Mac, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Prolog, VD1689_94/Ps, VD1689_94/Sak, VD1689_94/Zah, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr, Witt1702_PAN, Zv1681_Kok, Zv1681_Liec_1, Zv1689_Kan, Zv1698_Lig</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Asar, Apokr1689/Bar, Apokr1689/Bel, Apokr1689/GabpEst, Apokr1689/Jd, Apokr1689/Man, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Sus, Apokr1689/Tob, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Rm, JT1685/Tit, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
+  </si>
+  <si>
+    <t>Glueck1699_SBM</t>
+  </si>
+  <si>
+    <t>Baum1699_LVV, Baumb1795_WLWJD, CC1585, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Eid1701_KB, Eid1701_RA, Elg1621_GCG, Ench1586, Ench1615, EvEp1587, EvEp1615, Fuer1650_70_1ms, Fuer1650_70_2ms, Glueck1699_SBM, Hag1790_IM, JT1685/Prolog_Iev, JT1685/Prolog_Tit, LGL1685_K1, LGL1685_V5, LS1625, Lod1778_WTMD, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1643_44_Cat, Manc1643_44_LVM, Manc1643_LGL, Manc1643_Syr, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Ps1615, SKL1696_KB, SL1684, StendAJ1790_LSMP, StendGF1789_SL, UP1587, VD1689_94/Prolog, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr, Witt1702_PAN, Zv1638_VAR, Zv1681_Kok, Zv1681_Liec_1, Zv1681_Liec_2, Zv1689_Kan, Zv1689_Salsnes, Zv1698_Lig</t>
+  </si>
+  <si>
+    <t>Kaut kādi tukšumi? Normunda indeksācijas kods paredz, ka var būt sastopams @x{} bez iekavu satura.</t>
   </si>
 </sst>
 </file>
@@ -658,20 +664,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="109.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="50" style="2" customWidth="1"/>
@@ -689,7 +695,7 @@
         <v>52</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>54</v>
@@ -712,10 +718,10 @@
         <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>27</v>
@@ -726,16 +732,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>29</v>
@@ -746,36 +752,36 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="330" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="345" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -783,16 +789,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -806,10 +812,10 @@
         <v>34</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -823,10 +829,10 @@
         <v>35</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -840,10 +846,10 @@
         <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -857,47 +863,47 @@
         <v>37</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -911,234 +917,242 @@
         <v>40</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    </row>
+    <row r="19" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="B19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G19" s="1" t="s">
+      <c r="F20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="D23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" s="2" t="s">
+    </row>
+    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="345" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="318" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>75</v>
+      <c r="D30" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Vert failam lieto nevis viena burta kodu, bet izvērsumu pilnā vārdā.
</commit_message>
<xml_diff>
--- a/Docs/SENIE-kodi-no-ASCII-datiem.xlsx
+++ b/Docs/SENIE-kodi-no-ASCII-datiem.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="109">
   <si>
     <t>Elg1621_GCG, Manc1631_LVM, Manc1638_L, Manc1638_PhL, Manc1638_Run, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr</t>
   </si>
@@ -289,6 +289,60 @@
   </si>
   <si>
     <t>Kaut kādi tukšumi? Normunda indeksācijas kods paredz, ka var būt sastopams @x{} bez iekavu satura.</t>
+  </si>
+  <si>
+    <t>Sketch parametrs</t>
+  </si>
+  <si>
+    <t>sheet</t>
+  </si>
+  <si>
+    <t>title-even</t>
+  </si>
+  <si>
+    <t>title-odd</t>
+  </si>
+  <si>
+    <t>polish</t>
+  </si>
+  <si>
+    <t>french</t>
+  </si>
+  <si>
+    <t>estonian</t>
+  </si>
+  <si>
+    <t>flemish</t>
+  </si>
+  <si>
+    <t>greek</t>
+  </si>
+  <si>
+    <t>italian</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>remark</t>
+  </si>
+  <si>
+    <t>latin</t>
+  </si>
+  <si>
+    <t>aramaic</t>
+  </si>
+  <si>
+    <t>english</t>
+  </si>
+  <si>
+    <t>parallel</t>
+  </si>
+  <si>
+    <t>german</t>
+  </si>
+  <si>
+    <t>carry-over</t>
   </si>
 </sst>
 </file>
@@ -342,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -360,6 +414,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,494 +721,549 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="109.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="50" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="115.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="50" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="F3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="F4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="345" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="345" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E7" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E13" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="F15" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E16" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="F19" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E22" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E23" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F24" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E26" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E28" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="345" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="345" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E30" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atbilstoši Everitas teiktajam @o izlabots par @r (aramiešu valoda) un pārindeksēts attiecīgais fails.
</commit_message>
<xml_diff>
--- a/Docs/SENIE-kodi-no-ASCII-datiem.xlsx
+++ b/Docs/SENIE-kodi-no-ASCII-datiem.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="108">
   <si>
     <t>Elg1621_GCG, Manc1631_LVM, Manc1638_L, Manc1638_PhL, Manc1638_Run, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr</t>
   </si>
@@ -192,9 +192,6 @@
     <t>Apokr1689/2Mak, Apokr1689/Sir, JT1685/Apd, JT1685/Ef, JT1685/Jn, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Prolog_Iev, JT1685/Rm, LGL1685_V5, Manc1631_LVM, Manc1637_Sal, Manc1643_44_LVM, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
   </si>
   <si>
-    <t>EvEp1615, JT1685/Mk, Manc1643_44_LVM, Manc1643_LGL, VLH1685</t>
-  </si>
-  <si>
     <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Bar, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Tob, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Rm, JT1685/Tit, Lod1775_SEAPP, Manc1643_44_LVM, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
   </si>
   <si>
@@ -282,9 +279,6 @@
     <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Asar, Apokr1689/Bar, Apokr1689/Bel, Apokr1689/GabpEst, Apokr1689/Jd, Apokr1689/Man, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Sus, Apokr1689/Tob, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Rm, JT1685/Tit, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
   </si>
   <si>
-    <t>Glueck1699_SBM</t>
-  </si>
-  <si>
     <t>Baum1699_LVV, Baumb1795_WLWJD, CC1585, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Eid1701_KB, Eid1701_RA, Elg1621_GCG, Ench1586, Ench1615, EvEp1587, EvEp1615, Fuer1650_70_1ms, Fuer1650_70_2ms, Glueck1699_SBM, Hag1790_IM, JT1685/Prolog_Iev, JT1685/Prolog_Tit, LGL1685_K1, LGL1685_V5, LS1625, Lod1778_WTMD, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1643_44_Cat, Manc1643_44_LVM, Manc1643_LGL, Manc1643_Syr, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Ps1615, SKL1696_KB, SL1684, StendAJ1790_LSMP, StendGF1789_SL, UP1587, VD1689_94/Prolog, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr, Witt1702_PAN, Zv1638_VAR, Zv1681_Kok, Zv1681_Liec_1, Zv1681_Liec_2, Zv1689_Kan, Zv1689_Salsnes, Zv1698_Lig</t>
   </si>
   <si>
@@ -343,6 +337,9 @@
   </si>
   <si>
     <t>carry-over</t>
+  </si>
+  <si>
+    <t>EvEp1615, Glueck1699_SBM, JT1685/Mk, Manc1643_44_LVM, Manc1643_LGL, VLH1685</t>
   </si>
 </sst>
 </file>
@@ -732,8 +729,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="115.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
@@ -743,11 +740,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>25</v>
@@ -756,7 +753,7 @@
         <v>52</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>54</v>
@@ -769,11 +766,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="3">
         <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -782,104 +779,104 @@
         <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>93</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="345" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:8" ht="330" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>4</v>
@@ -888,18 +885,18 @@
         <v>34</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>6</v>
@@ -908,18 +905,18 @@
         <v>35</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>8</v>
@@ -928,18 +925,18 @@
         <v>36</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>10</v>
@@ -948,38 +945,38 @@
         <v>37</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="180" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>56</v>
@@ -988,18 +985,18 @@
         <v>39</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>53</v>
@@ -1008,105 +1005,102 @@
         <v>40</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>62</v>
+      <c r="B14" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="C15" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>41</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="C16" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="B17" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="165" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>57</v>
@@ -1115,52 +1109,52 @@
         <v>44</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>63</v>
+      <c r="B21" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>104</v>
-      </c>
       <c r="C22" s="2" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>46</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>10</v>
@@ -1169,102 +1163,102 @@
         <v>47</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>106</v>
-      </c>
       <c r="C24" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>64</v>
+      <c r="B25" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="C26" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>49</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="B27" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="D28" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="D29" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="345" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="330" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>50</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Html failu drukāšana bet nepareizajiem unikodiem.
</commit_message>
<xml_diff>
--- a/Docs/SENIE-kodi-no-ASCII-datiem.xlsx
+++ b/Docs/SENIE-kodi-no-ASCII-datiem.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20384"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!LaumasDoc\Git\senie\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617A31E9-C1A7-481D-A16A-E0180DA6DD94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6465"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="111">
   <si>
     <t>Elg1621_GCG, Manc1631_LVM, Manc1638_L, Manc1638_PhL, Manc1638_Run, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr</t>
   </si>
@@ -285,67 +291,76 @@
     <t>Kaut kādi tukšumi? Normunda indeksācijas kods paredz, ka var būt sastopams @x{} bez iekavu satura.</t>
   </si>
   <si>
-    <t>Sketch parametrs</t>
-  </si>
-  <si>
-    <t>sheet</t>
-  </si>
-  <si>
-    <t>title-even</t>
-  </si>
-  <si>
-    <t>title-odd</t>
-  </si>
-  <si>
-    <t>polish</t>
-  </si>
-  <si>
-    <t>french</t>
-  </si>
-  <si>
-    <t>estonian</t>
-  </si>
-  <si>
-    <t>flemish</t>
-  </si>
-  <si>
-    <t>greek</t>
-  </si>
-  <si>
-    <t>italian</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>remark</t>
-  </si>
-  <si>
-    <t>latin</t>
-  </si>
-  <si>
-    <t>aramaic</t>
-  </si>
-  <si>
-    <t>english</t>
-  </si>
-  <si>
-    <t>parallel</t>
-  </si>
-  <si>
-    <t>german</t>
-  </si>
-  <si>
-    <t>carry-over</t>
-  </si>
-  <si>
     <t>EvEp1615, Glueck1699_SBM, JT1685/Mk, Manc1643_44_LVM, Manc1643_LGL, VLH1685</t>
+  </si>
+  <si>
+    <t>Sheet</t>
+  </si>
+  <si>
+    <t>Title (even)</t>
+  </si>
+  <si>
+    <t>Title (odd)</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Carry-over</t>
+  </si>
+  <si>
+    <t>Polish</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>Estonian</t>
+  </si>
+  <si>
+    <t>Flemish</t>
+  </si>
+  <si>
+    <t>Greek</t>
+  </si>
+  <si>
+    <t>Italian</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Latin</t>
+  </si>
+  <si>
+    <t>Chapter ID</t>
+  </si>
+  <si>
+    <t>Nosaukums Sketch-ā un tooltip-os</t>
+  </si>
+  <si>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>Aramaic</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Parallel</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>Source ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -474,7 +489,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -507,9 +522,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -542,6 +574,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -717,7 +766,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
@@ -727,21 +776,21 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="115.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7265625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="5.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="115.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="50" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>24</v>
@@ -765,7 +814,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>90</v>
       </c>
@@ -788,7 +837,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>91</v>
       </c>
@@ -811,7 +860,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>92</v>
       </c>
@@ -834,7 +883,10 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="330" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -851,9 +903,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>2</v>
@@ -871,9 +923,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>3</v>
@@ -891,9 +943,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>5</v>
@@ -911,9 +963,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>7</v>
@@ -931,9 +983,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>9</v>
@@ -951,7 +1003,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="159.5" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
@@ -971,9 +1023,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>12</v>
@@ -991,9 +1043,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>13</v>
@@ -1011,7 +1063,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="s">
         <v>61</v>
       </c>
@@ -1022,9 +1074,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="145" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>14</v>
@@ -1042,9 +1094,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="145" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>15</v>
@@ -1062,12 +1114,15 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="145" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="B18" s="3" t="s">
         <v>16</v>
       </c>
@@ -1084,7 +1139,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
         <v>17</v>
       </c>
@@ -1095,9 +1150,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="145" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>18</v>
@@ -1121,7 +1176,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="s">
         <v>62</v>
       </c>
@@ -1129,15 +1184,15 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>46</v>
@@ -1149,9 +1204,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>20</v>
@@ -1169,9 +1224,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>21</v>
@@ -1189,7 +1244,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B25" s="3" t="s">
         <v>63</v>
       </c>
@@ -1197,9 +1252,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>22</v>
@@ -1217,12 +1272,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B27" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B28" s="3" t="s">
         <v>65</v>
       </c>
@@ -1236,7 +1291,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B29" s="3" t="s">
         <v>66</v>
       </c>
@@ -1244,7 +1299,10 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="330" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="B30" s="3" t="s">
         <v>23</v>
       </c>
@@ -1268,24 +1326,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Jaunais marķējums @0{...}, kas nozīmē izsvītrotu tekstu.
</commit_message>
<xml_diff>
--- a/Docs/SENIE-kodi-no-ASCII-datiem.xlsx
+++ b/Docs/SENIE-kodi-no-ASCII-datiem.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!LaumasDoc\Git\senie\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617A31E9-C1A7-481D-A16A-E0180DA6DD94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37021638-C007-4B73-AF8F-876DBEAF4EA0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="114">
   <si>
     <t>Elg1621_GCG, Manc1631_LVM, Manc1638_L, Manc1638_PhL, Manc1638_Run, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr</t>
   </si>
@@ -355,13 +355,22 @@
   </si>
   <si>
     <t>Source ID</t>
+  </si>
+  <si>
+    <t>izsvītrots teksts</t>
+  </si>
+  <si>
+    <t>Nē (Normunds/Lauma)</t>
+  </si>
+  <si>
+    <t>Strikethrough</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,6 +381,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -408,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -429,6 +445,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -767,18 +793,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" style="3" customWidth="1"/>
     <col min="2" max="2" width="5.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="115.54296875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.26953125" style="2" bestFit="1" customWidth="1"/>
@@ -814,64 +840,60 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:8" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="9">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="E3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="3">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>68</v>
@@ -880,61 +902,64 @@
         <v>69</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="3">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="304.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+    <row r="6" spans="1:8" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+    <row r="7" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>67</v>
@@ -945,16 +970,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>67</v>
@@ -965,16 +990,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>67</v>
@@ -985,110 +1010,110 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="B11" s="3" t="s">
+      <c r="E11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F11" s="2" t="s">
+      <c r="E12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B14" s="3" t="s">
+      <c r="E14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B15" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="145" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>69</v>
@@ -1096,226 +1121,246 @@
     </row>
     <row r="16" spans="1:8" ht="145" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="145" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B17" s="3" t="s">
+      <c r="E17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B18" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="145" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+    <row r="19" spans="1:8" ht="145" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="2" t="s">
+      <c r="E19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B19" s="3" t="s">
+    <row r="20" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="145" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
+      <c r="F20" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="145" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B21" s="3" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B22" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B24" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
+      <c r="E24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B25" s="3" t="s">
+      <c r="F25" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B26" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
+    <row r="27" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B27" s="3" t="s">
+      <c r="E27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B28" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B28" s="3" t="s">
+    <row r="29" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B29" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B29" s="3" t="s">
+      <c r="E29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B30" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="304.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
+    <row r="31" spans="1:8" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B31" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F30" s="2" t="s">
+      <c r="E31" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>